<commit_message>
Updated GemBox.Spreadsheet example projects.
</commit_message>
<xml_diff>
--- a/C#/Advanced Features/Html Export/HtmlExport.xlsx
+++ b/C#/Advanced Features/Html Export/HtmlExport.xlsx
@@ -1,28 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stipo\Gemmeus Repo\ExampleExplorer\GemBox.ExampleExplorer.Web\Examples\Spreadsheet\[Common]\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ECHO\MyGemBoxGit\ExampleExplorer\GemBox.ExampleExplorer.Web\Examples\Spreadsheet\[Common]\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{793AE688-B323-4E81-BA91-9EDB72D61D4F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683F3BA1-DBF7-4959-82D7-070E5824ED43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Typical Table" sheetId="1" r:id="rId1"/>
     <sheet name="Simple Sheet" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="68">
   <si>
     <t>Rank</t>
   </si>
@@ -196,6 +195,36 @@
   </si>
   <si>
     <t>Example of table - tallest buildings in the world (2019):</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>$3,600</t>
+  </si>
+  <si>
+    <t>Fred Nurk</t>
+  </si>
+  <si>
+    <t>$2,580</t>
+  </si>
+  <si>
+    <t>Hans Meier</t>
+  </si>
+  <si>
+    <t>$3,200</t>
+  </si>
+  <si>
+    <t>Ivan Horvat</t>
+  </si>
+  <si>
+    <t>$4,100</t>
   </si>
 </sst>
 </file>
@@ -206,7 +235,7 @@
     <numFmt numFmtId="164" formatCode="#&quot; m&quot;"/>
     <numFmt numFmtId="165" formatCode="#&quot; ft&quot;"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,6 +257,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -263,7 +300,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -408,11 +445,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -437,6 +484,12 @@
     <xf numFmtId="164" fontId="2" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -473,14 +526,15 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -862,42 +916,42 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="D21" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="22" t="s">
+      <c r="E21" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22" t="s">
+      <c r="F21" s="24"/>
+      <c r="G21" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="H21" s="24" t="s">
+      <c r="H21" s="26" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="35"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
       <c r="E22" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G22" s="23"/>
-      <c r="H22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="27"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
@@ -924,10 +978,10 @@
       <c r="H23" s="6">
         <v>2010</v>
       </c>
-      <c r="I23" s="26" t="s">
+      <c r="I23" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="J23" s="29" t="s">
+      <c r="J23" s="31" t="s">
         <v>13</v>
       </c>
     </row>
@@ -956,8 +1010,8 @@
       <c r="H24" s="11">
         <v>2015</v>
       </c>
-      <c r="I24" s="27"/>
-      <c r="J24" s="30"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="32"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
@@ -984,8 +1038,8 @@
       <c r="H25" s="16">
         <v>2012</v>
       </c>
-      <c r="I25" s="27"/>
-      <c r="J25" s="30"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="32"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
@@ -1012,8 +1066,8 @@
       <c r="H26" s="11">
         <v>2017</v>
       </c>
-      <c r="I26" s="27"/>
-      <c r="J26" s="30"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="32"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
@@ -1040,8 +1094,8 @@
       <c r="H27" s="16">
         <v>2016</v>
       </c>
-      <c r="I27" s="27"/>
-      <c r="J27" s="30"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="32"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
@@ -1068,8 +1122,8 @@
       <c r="H28" s="11">
         <v>2014</v>
       </c>
-      <c r="I28" s="27"/>
-      <c r="J28" s="30"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
@@ -1096,8 +1150,8 @@
       <c r="H29" s="16">
         <v>2016</v>
       </c>
-      <c r="I29" s="27"/>
-      <c r="J29" s="30"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="32"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
@@ -1124,8 +1178,8 @@
       <c r="H30" s="11">
         <v>2018</v>
       </c>
-      <c r="I30" s="27"/>
-      <c r="J30" s="30"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="32"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
@@ -1152,8 +1206,8 @@
       <c r="H31" s="16">
         <v>2018</v>
       </c>
-      <c r="I31" s="27"/>
-      <c r="J31" s="30"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="32"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="17">
@@ -1180,8 +1234,8 @@
       <c r="H32" s="21">
         <v>2004</v>
       </c>
-      <c r="I32" s="28"/>
-      <c r="J32" s="30"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="32"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
@@ -1208,8 +1262,8 @@
       <c r="H33" s="16">
         <v>2008</v>
       </c>
-      <c r="I33" s="32"/>
-      <c r="J33" s="30"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="32"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
@@ -1236,8 +1290,8 @@
       <c r="H34" s="11">
         <v>2010</v>
       </c>
-      <c r="I34" s="32"/>
-      <c r="J34" s="30"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="32"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
@@ -1264,8 +1318,8 @@
       <c r="H35" s="16">
         <v>2018</v>
       </c>
-      <c r="I35" s="32"/>
-      <c r="J35" s="30"/>
+      <c r="I35" s="34"/>
+      <c r="J35" s="32"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
@@ -1292,8 +1346,8 @@
       <c r="H36" s="11">
         <v>2018</v>
       </c>
-      <c r="I36" s="32"/>
-      <c r="J36" s="30"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="32"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
@@ -1320,8 +1374,8 @@
       <c r="H37" s="16">
         <v>2017</v>
       </c>
-      <c r="I37" s="32"/>
-      <c r="J37" s="30"/>
+      <c r="I37" s="34"/>
+      <c r="J37" s="32"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
@@ -1348,8 +1402,8 @@
       <c r="H38" s="11">
         <v>1998</v>
       </c>
-      <c r="I38" s="32"/>
-      <c r="J38" s="30"/>
+      <c r="I38" s="34"/>
+      <c r="J38" s="32"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
@@ -1376,8 +1430,8 @@
       <c r="H39" s="16">
         <v>1998</v>
       </c>
-      <c r="I39" s="32"/>
-      <c r="J39" s="30"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="32"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
@@ -1404,8 +1458,8 @@
       <c r="H40" s="11">
         <v>2018</v>
       </c>
-      <c r="I40" s="32"/>
-      <c r="J40" s="30"/>
+      <c r="I40" s="34"/>
+      <c r="J40" s="32"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
@@ -1432,8 +1486,8 @@
       <c r="H41" s="16">
         <v>2010</v>
       </c>
-      <c r="I41" s="32"/>
-      <c r="J41" s="30"/>
+      <c r="I41" s="34"/>
+      <c r="J41" s="32"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="17">
@@ -1460,21 +1514,21 @@
       <c r="H42" s="21">
         <v>2017</v>
       </c>
-      <c r="I42" s="33"/>
-      <c r="J42" s="31"/>
+      <c r="I42" s="35"/>
+      <c r="J42" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="I23:I32"/>
+    <mergeCell ref="J23:J42"/>
+    <mergeCell ref="I33:I42"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="I23:I32"/>
-    <mergeCell ref="J23:J42"/>
-    <mergeCell ref="I33:I42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1484,49 +1538,58 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24C9F10A-350D-4548-B3B8-B5AB1CFE05FB}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <v>2</v>
-      </c>
-      <c r="C1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93936B43-9577-4E73-BC71-A788D8669B34}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="36" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="36" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>